<commit_message>
New Changes to integrate with the SWS
</commit_message>
<xml_diff>
--- a/data-raw/VariableDescription_18July17_AEE.xlsx
+++ b/data-raw/VariableDescription_18July17_AEE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Team_working_folder\A\GFLI\2_Estimation-Methods\SWS_LossModule\variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENGLISHA\Documents\faoswsLoss\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$A$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$X$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$Y$103</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="565">
   <si>
     <t>Foreign Matter</t>
   </si>
@@ -1570,6 +1570,237 @@
   </si>
   <si>
     <t>Index Related</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>Investment_ConsumptionFixedCapital</t>
+  </si>
+  <si>
+    <t>Investment_GrossCapitalStocks</t>
+  </si>
+  <si>
+    <t>Investment_GrossFixedCapitalFormation_USD</t>
+  </si>
+  <si>
+    <t>CredittoAg</t>
+  </si>
+  <si>
+    <t>Sankey_Diagram_IEA20Apr17</t>
+  </si>
+  <si>
+    <t>CMOHistoricalDataAnnual_sh1</t>
+  </si>
+  <si>
+    <t>IronSteelIMport7055475</t>
+  </si>
+  <si>
+    <t>Rain_climate</t>
+  </si>
+  <si>
+    <t>Temp_climate</t>
+  </si>
+  <si>
+    <t>WP_time_01_9</t>
+  </si>
+  <si>
+    <t>WP_time_01_8</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_OR_ZS</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_R1_ZS</t>
+  </si>
+  <si>
+    <t>SI_DST_02ND_20</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_WR_ZS</t>
+  </si>
+  <si>
+    <t>SI_DST_03RD_20</t>
+  </si>
+  <si>
+    <t>SI_DST_FRST_20</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_WR_ZS</t>
+  </si>
+  <si>
+    <t>BX_KLT_DREM_CD_DT</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_PC_CD</t>
+  </si>
+  <si>
+    <t>SI_DST_FRST_10</t>
+  </si>
+  <si>
+    <t>BN_TRF_CURR_CD</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_OR_ZS</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R1_ZS</t>
+  </si>
+  <si>
+    <t>BM_GSR_TOTL_CD</t>
+  </si>
+  <si>
+    <t>BX_TRF_CURR_CD</t>
+  </si>
+  <si>
+    <t>BM_GSR_FCTY_CD</t>
+  </si>
+  <si>
+    <t>BX_GSR_TOTL_CD</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_R5_ZS</t>
+  </si>
+  <si>
+    <t>SI_DST_04TH_20</t>
+  </si>
+  <si>
+    <t>BX_GSR_FCTY_CD</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R5_ZS</t>
+  </si>
+  <si>
+    <t>BN_GSR_FCTY_CD</t>
+  </si>
+  <si>
+    <t>EG_ELC_ACCS_ZS</t>
+  </si>
+  <si>
+    <t>BM_TRF_PRVT_CD</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_R2_ZS</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_PC_KD</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R2_ZS</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_PC_KD_ZG</t>
+  </si>
+  <si>
+    <t>NY_GSR_NFCY_KN</t>
+  </si>
+  <si>
+    <t>NY_GSR_NFCY_CD</t>
+  </si>
+  <si>
+    <t>NY_GSR_NFCY_CN</t>
+  </si>
+  <si>
+    <t>WP15163_4_8</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_KD_ZG</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R4_ZS</t>
+  </si>
+  <si>
+    <t>SI_SPR_PCAP_ZG</t>
+  </si>
+  <si>
+    <t>GC_TAX_YPKG_CN</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_CD</t>
+  </si>
+  <si>
+    <t>WP15163_4_9</t>
+  </si>
+  <si>
+    <t>GC_TAX_YPKG_ZS</t>
+  </si>
+  <si>
+    <t>DT_DOD_PVLX_EX_ZS</t>
+  </si>
+  <si>
+    <t>NY_GDY_TOTL_KN</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R3_ZS</t>
+  </si>
+  <si>
+    <t>DT_ODA_ODAT_MP_ZS</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_R6_ZS</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_R3_ZS</t>
+  </si>
+  <si>
+    <t>GC_TAX_YPKG_RV_ZS</t>
+  </si>
+  <si>
+    <t>SI_SPR_PC40_ZG</t>
+  </si>
+  <si>
+    <t>NY_ADJ_NNTY_KD</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_R6_ZS</t>
+  </si>
+  <si>
+    <t>TX_VAL_MRCH_HI_ZS</t>
+  </si>
+  <si>
+    <t>SI_SPR_PCAP</t>
+  </si>
+  <si>
+    <t>SI_SPR_PC40</t>
+  </si>
+  <si>
+    <t>TM_VAL_MRCH_HI_ZS</t>
+  </si>
+  <si>
+    <t>SI_DST_10TH_10</t>
+  </si>
+  <si>
+    <t>SI_DST_05TH_20</t>
+  </si>
+  <si>
+    <t>DT_DOD_DSTC_XP_ZS</t>
+  </si>
+  <si>
+    <t>DT_DOD_DECT_EX_ZS</t>
+  </si>
+  <si>
+    <t>DT_TDS_DECT_EX_ZS</t>
+  </si>
+  <si>
+    <t>DT_TDS_DPPG_XP_ZS</t>
+  </si>
+  <si>
+    <t>DT_INT_DECT_EX_ZS</t>
+  </si>
+  <si>
+    <t>DT_TDS_DPPF_XP_ZS</t>
+  </si>
+  <si>
+    <t>Investment_NetCapitalStocks</t>
+  </si>
+  <si>
+    <t>LPIDATA</t>
+  </si>
+  <si>
+    <t>Top10_GrossProductionValue</t>
+  </si>
+  <si>
+    <t>Top10_Foodsupplykcal</t>
   </si>
 </sst>
 </file>
@@ -1952,12 +2183,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X113"/>
+  <dimension ref="A1:Y113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
+      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1967,12 +2198,12 @@
     <col min="3" max="3" width="61.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="6" width="18.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="8" width="46" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1995,55 +2226,58 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>382</v>
       </c>
@@ -2063,25 +2297,28 @@
       <c r="G2" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>335</v>
       </c>
@@ -2101,20 +2338,23 @@
       <c r="G3" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>335</v>
       </c>
@@ -2134,20 +2374,23 @@
       <c r="G4" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>335</v>
       </c>
@@ -2167,26 +2410,29 @@
       <c r="G5" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>375</v>
       </c>
@@ -2206,27 +2452,30 @@
       <c r="G6" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="4"/>
+      <c r="N6" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>335</v>
       </c>
@@ -2246,20 +2495,23 @@
       <c r="G7" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>375</v>
       </c>
@@ -2279,26 +2531,29 @@
       <c r="G8" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="5"/>
+      <c r="N8" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="5"/>
+      <c r="P8" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>335</v>
       </c>
@@ -2318,20 +2573,23 @@
       <c r="G9" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>382</v>
       </c>
@@ -2353,17 +2611,20 @@
       <c r="G10" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>318</v>
       </c>
@@ -2386,37 +2647,40 @@
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>318</v>
       </c>
@@ -2439,31 +2703,34 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>382</v>
       </c>
@@ -2485,17 +2752,20 @@
       <c r="G13" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>316</v>
       </c>
@@ -2518,40 +2788,43 @@
         <v>32</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>318</v>
       </c>
@@ -2574,37 +2847,40 @@
         <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="W15" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>382</v>
       </c>
@@ -2626,17 +2902,20 @@
       <c r="G16" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="P16" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>316</v>
       </c>
@@ -2659,40 +2938,43 @@
         <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="W17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>316</v>
       </c>
@@ -2715,40 +2997,43 @@
         <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>318</v>
       </c>
@@ -2771,37 +3056,40 @@
         <v>32</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="W19" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2824,28 +3112,31 @@
         <v>32</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>316</v>
       </c>
@@ -2868,28 +3159,31 @@
         <v>32</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>316</v>
       </c>
@@ -2912,40 +3206,43 @@
         <v>32</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>316</v>
       </c>
@@ -2968,37 +3265,40 @@
         <v>32</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="V23" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="W23" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="X23" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>318</v>
       </c>
@@ -3021,37 +3321,40 @@
         <v>32</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="V24" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="W24" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>318</v>
       </c>
@@ -3074,31 +3377,34 @@
         <v>32</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>382</v>
       </c>
@@ -3120,17 +3426,20 @@
       <c r="G26" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="O26" s="4" t="s">
+      <c r="P26" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>318</v>
       </c>
@@ -3153,31 +3462,34 @@
         <v>32</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -3200,31 +3512,34 @@
         <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>316</v>
       </c>
@@ -3247,31 +3562,34 @@
         <v>32</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="X29" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>318</v>
       </c>
@@ -3294,31 +3612,34 @@
         <v>32</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="X30" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>318</v>
       </c>
@@ -3341,31 +3662,34 @@
         <v>32</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>316</v>
       </c>
@@ -3388,40 +3712,43 @@
         <v>32</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U32" s="1" t="s">
+      <c r="V32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V32" s="1" t="s">
+      <c r="W32" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W32" s="1" t="s">
+      <c r="X32" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>316</v>
       </c>
@@ -3444,31 +3771,34 @@
         <v>32</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="W33" s="1" t="s">
+      <c r="X33" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>318</v>
       </c>
@@ -3491,31 +3821,34 @@
         <v>32</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>316</v>
       </c>
@@ -3538,37 +3871,40 @@
         <v>32</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="U35" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="V35" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="V35" s="1" t="s">
+      <c r="W35" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="W35" s="1" t="s">
+      <c r="X35" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>321</v>
       </c>
@@ -3591,34 +3927,37 @@
         <v>32</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U36" s="1" t="s">
+      <c r="V36" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -3641,31 +3980,34 @@
         <v>32</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="W37" s="1" t="s">
+      <c r="X37" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>318</v>
       </c>
@@ -3688,31 +4030,34 @@
         <v>32</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>316</v>
       </c>
@@ -3735,31 +4080,34 @@
         <v>32</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="R39" s="1">
         <v>2010</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>318</v>
       </c>
@@ -3782,31 +4130,34 @@
         <v>32</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>333</v>
       </c>
@@ -3828,20 +4179,23 @@
       <c r="G41" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="I41" t="s">
         <v>441</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>426</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="Q41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>316</v>
       </c>
@@ -3864,28 +4218,31 @@
         <v>32</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P42" s="1" t="s">
+      <c r="Q42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>320</v>
       </c>
@@ -3908,28 +4265,31 @@
         <v>32</v>
       </c>
       <c r="H43" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="Q43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>320</v>
       </c>
@@ -3952,25 +4312,28 @@
         <v>32</v>
       </c>
       <c r="H44" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>333</v>
       </c>
@@ -3992,20 +4355,23 @@
       <c r="G45" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="I45" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>426</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="Q45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>320</v>
       </c>
@@ -4028,25 +4394,28 @@
         <v>32</v>
       </c>
       <c r="H46" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="Q46" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>319</v>
       </c>
@@ -4069,31 +4438,34 @@
         <v>32</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P47" s="1" t="s">
+      <c r="Q47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R47" s="1">
+      <c r="S47" s="1">
         <v>2014</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>333</v>
       </c>
@@ -4115,20 +4487,23 @@
       <c r="G48" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="I48" t="s">
         <v>443</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="O48" t="s">
+      <c r="P48" t="s">
         <v>426</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="Q48" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>316</v>
       </c>
@@ -4151,37 +4526,40 @@
         <v>32</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="N49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P49" s="1" t="s">
+      <c r="Q49" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T49" s="1" t="s">
+      <c r="U49" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U49" s="1" t="s">
+      <c r="V49" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V49" s="1" t="s">
+      <c r="W49" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>318</v>
       </c>
@@ -4204,31 +4582,34 @@
         <v>32</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P50" s="1" t="s">
+      <c r="Q50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="T50" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>316</v>
       </c>
@@ -4251,40 +4632,43 @@
         <v>32</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O51" s="1" t="s">
+      <c r="P51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V51" s="1" t="s">
+      <c r="W51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="W51" s="1" t="s">
+      <c r="X51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="X51" s="1" t="s">
+      <c r="Y51" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>316</v>
       </c>
@@ -4307,31 +4691,34 @@
         <v>32</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="N52" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="P52" s="1" t="s">
+      <c r="Q52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T52" s="1" t="s">
+      <c r="U52" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="V52" s="1" t="s">
+      <c r="W52" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>316</v>
       </c>
@@ -4354,37 +4741,40 @@
         <v>32</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="Q53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S53" s="1" t="s">
+      <c r="T53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T53" s="1" t="s">
+      <c r="U53" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U53" s="1" t="s">
+      <c r="V53" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V53" s="1" t="s">
+      <c r="W53" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>335</v>
       </c>
@@ -4406,17 +4796,20 @@
       <c r="G54" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H54" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="K54" s="6" t="s">
+      <c r="L54" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="O54" s="4" t="s">
+      <c r="P54" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>333</v>
       </c>
@@ -4438,20 +4831,23 @@
       <c r="G55" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I55" t="s">
         <v>442</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>426</v>
       </c>
-      <c r="P55" s="1" t="s">
+      <c r="Q55" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>319</v>
       </c>
@@ -4474,31 +4870,34 @@
         <v>32</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="M56" s="1" t="s">
+      <c r="N56" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P56" s="1" t="s">
+      <c r="Q56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R56" s="1">
+      <c r="S56" s="1">
         <v>2014</v>
       </c>
-      <c r="S56" s="1" t="s">
+      <c r="T56" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>316</v>
       </c>
@@ -4521,31 +4920,34 @@
         <v>32</v>
       </c>
       <c r="H57" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="N57" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N57" s="1" t="s">
+      <c r="O57" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="P57" s="1" t="s">
+      <c r="Q57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T57" s="1" t="s">
+      <c r="U57" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="V57" s="1" t="s">
+      <c r="W57" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -4568,34 +4970,37 @@
         <v>32</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="N58" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N58" s="1" t="s">
+      <c r="O58" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P58" s="1" t="s">
+      <c r="Q58" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T58" s="1" t="s">
+      <c r="U58" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="U58" s="1" t="s">
+      <c r="V58" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="V58" s="1" t="s">
+      <c r="W58" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>316</v>
       </c>
@@ -4618,28 +5023,31 @@
         <v>32</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="N59" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N59" s="1" t="s">
+      <c r="O59" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P59" s="1" t="s">
+      <c r="Q59" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q59" s="1" t="s">
+      <c r="R59" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>318</v>
       </c>
@@ -4662,31 +5070,34 @@
         <v>32</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="M60" s="1" t="s">
+      <c r="N60" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N60" s="1" t="s">
+      <c r="O60" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P60" s="1" t="s">
+      <c r="Q60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S60" s="1" t="s">
+      <c r="T60" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>320</v>
       </c>
@@ -4709,28 +5120,31 @@
         <v>32</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M61" s="1" t="s">
+      <c r="N61" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N61" s="1" t="s">
+      <c r="O61" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P61" s="1" t="s">
+      <c r="Q61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S61" s="1" t="s">
+      <c r="T61" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>320</v>
       </c>
@@ -4753,28 +5167,31 @@
         <v>32</v>
       </c>
       <c r="H62" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M62" s="1" t="s">
+      <c r="N62" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N62" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P62" s="1" t="s">
+      <c r="Q62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S62" s="1" t="s">
+      <c r="T62" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -4797,40 +5214,43 @@
         <v>32</v>
       </c>
       <c r="H63" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="L63" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="N63" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="N63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="P63" s="1" t="s">
+      <c r="Q63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S63" s="1" t="s">
+      <c r="T63" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T63" s="1" t="s">
+      <c r="U63" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="U63" s="1" t="s">
+      <c r="V63" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="V63" s="1" t="s">
+      <c r="W63" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>318</v>
       </c>
@@ -4853,31 +5273,34 @@
         <v>32</v>
       </c>
       <c r="H64" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J64" s="1" t="s">
+      <c r="K64" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="M64" s="1" t="s">
+      <c r="N64" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N64" s="1" t="s">
+      <c r="O64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P64" s="1" t="s">
+      <c r="Q64" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S64" s="1" t="s">
+      <c r="T64" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>318</v>
       </c>
@@ -4900,31 +5323,34 @@
         <v>32</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M65" s="1" t="s">
+      <c r="N65" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N65" s="1" t="s">
+      <c r="O65" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P65" s="1" t="s">
+      <c r="Q65" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S65" s="1" t="s">
+      <c r="T65" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>316</v>
       </c>
@@ -4947,34 +5373,37 @@
         <v>32</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="K66" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="M66" s="1" t="s">
+      <c r="N66" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="P66" s="1" t="s">
+      <c r="Q66" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S66" s="1" t="s">
+      <c r="T66" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="T66" s="1" t="s">
+      <c r="U66" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="V66" s="1" t="s">
+      <c r="W66" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>316</v>
       </c>
@@ -4997,40 +5426,43 @@
         <v>32</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="L67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M67" s="1" t="s">
+      <c r="N67" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N67" s="1" t="s">
+      <c r="O67" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O67" s="1" t="s">
+      <c r="P67" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P67" s="1" t="s">
+      <c r="Q67" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V67" s="1" t="s">
+      <c r="W67" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="W67" s="1" t="s">
+      <c r="X67" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="X67" s="1" t="s">
+      <c r="Y67" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>316</v>
       </c>
@@ -5053,40 +5485,43 @@
         <v>32</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="J68" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M68" s="1" t="s">
+      <c r="N68" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N68" s="1" t="s">
+      <c r="O68" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P68" s="1" t="s">
+      <c r="Q68" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q68" s="1">
+      <c r="R68" s="1">
         <v>2010</v>
       </c>
-      <c r="S68" s="1" t="s">
+      <c r="T68" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T68" s="1" t="s">
+      <c r="U68" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U68" s="1" t="s">
+      <c r="V68" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V68" s="1" t="s">
+      <c r="W68" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>318</v>
       </c>
@@ -5109,31 +5544,34 @@
         <v>32</v>
       </c>
       <c r="H69" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="L69" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="N69" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N69" s="1" t="s">
+      <c r="O69" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P69" s="1" t="s">
+      <c r="Q69" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S69" s="1" t="s">
+      <c r="T69" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>318</v>
       </c>
@@ -5156,37 +5594,40 @@
         <v>32</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M70" s="1" t="s">
+      <c r="N70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N70" s="1" t="s">
+      <c r="O70" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P70" s="1" t="s">
+      <c r="Q70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S70" s="1" t="s">
+      <c r="T70" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U70" s="1" t="s">
+      <c r="V70" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="V70" s="1" t="s">
+      <c r="W70" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>316</v>
       </c>
@@ -5209,37 +5650,40 @@
         <v>32</v>
       </c>
       <c r="H71" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="M71" s="1" t="s">
+      <c r="N71" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N71" s="1" t="s">
+      <c r="O71" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O71" s="1" t="s">
+      <c r="P71" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="P71" s="1" t="s">
+      <c r="Q71" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V71" s="1" t="s">
+      <c r="W71" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="W71" s="1" t="s">
+      <c r="X71" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="X71" s="1" t="s">
+      <c r="Y71" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>316</v>
       </c>
@@ -5262,37 +5706,40 @@
         <v>32</v>
       </c>
       <c r="H72" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="J72" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="K72" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="M72" s="1" t="s">
+      <c r="N72" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N72" s="1" t="s">
+      <c r="O72" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O72" s="1" t="s">
+      <c r="P72" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="P72" s="1" t="s">
+      <c r="Q72" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V72" s="1" t="s">
+      <c r="W72" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="W72" s="1" t="s">
+      <c r="X72" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="X72" s="1" t="s">
+      <c r="Y72" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>335</v>
       </c>
@@ -5314,17 +5761,20 @@
       <c r="G73" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H73" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I73" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="K73" s="6" t="s">
+      <c r="L73" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="O73" s="4" t="s">
+      <c r="P73" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>318</v>
       </c>
@@ -5347,37 +5797,40 @@
         <v>32</v>
       </c>
       <c r="H74" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="K74" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="M74" s="1" t="s">
+      <c r="N74" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N74" s="1" t="s">
+      <c r="O74" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="P74" s="1" t="s">
+      <c r="Q74" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S74" s="1" t="s">
+      <c r="T74" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U74" s="1" t="s">
+      <c r="V74" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="V74" s="1" t="s">
+      <c r="W74" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>316</v>
       </c>
@@ -5400,40 +5853,43 @@
         <v>32</v>
       </c>
       <c r="H75" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="K75" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="N75" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N75" s="1" t="s">
+      <c r="O75" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O75" s="1" t="s">
+      <c r="P75" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P75" s="1" t="s">
+      <c r="Q75" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T75" s="1" t="s">
+      <c r="U75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U75" s="1" t="s">
+      <c r="V75" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V75" s="1" t="s">
+      <c r="W75" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W75" s="1" t="s">
+      <c r="X75" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>316</v>
       </c>
@@ -5456,40 +5912,43 @@
         <v>32</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M76" s="1" t="s">
+      <c r="N76" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N76" s="1" t="s">
+      <c r="O76" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O76" s="1" t="s">
+      <c r="P76" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P76" s="1" t="s">
+      <c r="Q76" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T76" s="1" t="s">
+      <c r="U76" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U76" s="1" t="s">
+      <c r="V76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V76" s="1" t="s">
+      <c r="W76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W76" s="1" t="s">
+      <c r="X76" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -5512,28 +5971,31 @@
         <v>32</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="I77" s="1" t="s">
+      <c r="J77" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="K77" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="M77" s="1" t="s">
+      <c r="N77" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N77" s="1" t="s">
+      <c r="O77" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P77" s="1" t="s">
+      <c r="Q77" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S77" s="1" t="s">
+      <c r="T77" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>335</v>
       </c>
@@ -5555,17 +6017,20 @@
       <c r="G78" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H78" s="4" t="s">
+      <c r="H78" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I78" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="K78" s="6" t="s">
+      <c r="L78" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="O78" s="4" t="s">
+      <c r="P78" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -5588,28 +6053,31 @@
         <v>32</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="J79" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J79" s="1" t="s">
+      <c r="K79" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M79" s="1" t="s">
+      <c r="N79" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N79" s="1" t="s">
+      <c r="O79" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P79" s="1" t="s">
+      <c r="Q79" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S79" s="1" t="s">
+      <c r="T79" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>335</v>
       </c>
@@ -5631,17 +6099,20 @@
       <c r="G80" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="H80" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="K80" s="6" t="s">
+      <c r="L80" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="O80" s="4" t="s">
+      <c r="P80" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -5664,37 +6135,40 @@
         <v>32</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="I81" s="1" t="s">
+      <c r="J81" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J81" s="1" t="s">
+      <c r="K81" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="N81" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N81" s="1" t="s">
+      <c r="O81" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P81" s="1" t="s">
+      <c r="Q81" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S81" s="1" t="s">
+      <c r="T81" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T81" s="1" t="s">
+      <c r="U81" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="U81" s="1" t="s">
+      <c r="V81" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="V81" s="1" t="s">
+      <c r="W81" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>335</v>
       </c>
@@ -5716,17 +6190,20 @@
       <c r="G82" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H82" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="K82" s="6" t="s">
+      <c r="L82" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="O82" s="4" t="s">
+      <c r="P82" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -5749,28 +6226,31 @@
         <v>32</v>
       </c>
       <c r="H83" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="I83" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I83" s="1" t="s">
+      <c r="J83" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J83" s="1" t="s">
+      <c r="K83" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="M83" s="1" t="s">
+      <c r="N83" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="N83" s="1" t="s">
+      <c r="O83" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P83" s="1" t="s">
+      <c r="Q83" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S83" s="1" t="s">
+      <c r="T83" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -5793,28 +6273,31 @@
         <v>32</v>
       </c>
       <c r="H84" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I84" s="1" t="s">
+      <c r="J84" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J84" s="1" t="s">
+      <c r="K84" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="N84" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N84" s="1" t="s">
+      <c r="O84" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P84" s="1" t="s">
+      <c r="Q84" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S84" s="1" t="s">
+      <c r="T84" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -5837,31 +6320,34 @@
         <v>32</v>
       </c>
       <c r="H85" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="I85" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I85" s="1" t="s">
+      <c r="J85" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J85" s="1" t="s">
+      <c r="K85" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K85" s="1" t="s">
+      <c r="L85" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M85" s="1" t="s">
+      <c r="N85" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N85" s="1" t="s">
+      <c r="O85" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P85" s="1" t="s">
+      <c r="Q85" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S85" s="1" t="s">
+      <c r="T85" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>335</v>
       </c>
@@ -5883,17 +6369,20 @@
       <c r="G86" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H86" s="4" t="s">
+      <c r="H86" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I86" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="K86" s="6" t="s">
+      <c r="L86" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="O86" s="4" t="s">
+      <c r="P86" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>26</v>
       </c>
@@ -5915,11 +6404,14 @@
       <c r="H87" t="s">
         <v>419</v>
       </c>
-      <c r="O87" s="1" t="s">
+      <c r="I87" t="s">
+        <v>419</v>
+      </c>
+      <c r="P87" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>335</v>
       </c>
@@ -5940,22 +6432,25 @@
         <v>405</v>
       </c>
       <c r="H88" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="I88" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="L88" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="M88" s="1" t="s">
+      <c r="N88" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="O88" s="1" t="s">
+      <c r="P88" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="P88" s="1" t="s">
+      <c r="Q88" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -5975,17 +6470,20 @@
       <c r="G89" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I89" t="s">
         <v>418</v>
       </c>
-      <c r="K89" s="7" t="s">
+      <c r="L89" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="O89" t="s">
+      <c r="P89" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>421</v>
       </c>
@@ -6005,20 +6503,23 @@
       <c r="G90" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="H90" s="10" t="s">
+      <c r="H90" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="I90" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="K90" s="7" t="s">
+      <c r="L90" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="O90" s="7" t="s">
+      <c r="P90" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="P90" s="7" t="s">
+      <c r="Q90" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="91" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>421</v>
       </c>
@@ -6035,23 +6536,26 @@
       <c r="F91" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="G91" s="7" t="s">
+      <c r="G91" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="I91" t="s">
         <v>433</v>
       </c>
-      <c r="K91" s="7" t="s">
+      <c r="L91" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>434</v>
       </c>
-      <c r="P91" s="7" t="s">
+      <c r="Q91" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>453</v>
       </c>
@@ -6071,17 +6575,20 @@
       <c r="G92" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H92" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="I92" t="s">
         <v>448</v>
       </c>
-      <c r="K92" s="7" t="s">
+      <c r="L92" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="O92" s="7" t="s">
+      <c r="P92" s="7" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="93" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>453</v>
       </c>
@@ -6099,11 +6606,14 @@
         <v>412</v>
       </c>
       <c r="G93" s="11"/>
-      <c r="M93" s="7" t="s">
+      <c r="H93" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="N93" s="7" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>453</v>
       </c>
@@ -6119,14 +6629,14 @@
       <c r="F94" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="M94" s="1" t="s">
+      <c r="N94" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>453</v>
       </c>
@@ -6142,14 +6652,14 @@
       <c r="F95" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="H95" s="1" t="s">
+      <c r="I95" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="M95" s="1" t="s">
+      <c r="N95" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>453</v>
       </c>
@@ -6171,8 +6681,11 @@
       <c r="H96" s="1" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>453</v>
       </c>
@@ -6191,11 +6704,14 @@
       <c r="G97" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="I97" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>453</v>
       </c>
@@ -6214,11 +6730,14 @@
       <c r="G98" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I98" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>453</v>
       </c>
@@ -6238,7 +6757,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>453</v>
       </c>
@@ -6258,7 +6777,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>453</v>
       </c>
@@ -6278,7 +6797,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>487</v>
       </c>
@@ -6297,8 +6816,11 @@
       <c r="G102" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H102" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>487</v>
       </c>
@@ -6317,49 +6839,53 @@
       <c r="G103" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C104" s="7"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C105" s="7"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C106" s="7"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C107" s="7"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C108" s="7"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C109" s="7"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C110" s="7"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C111" s="7"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C112" s="7"/>
     </row>
-    <row r="113" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C113" s="7"/>
       <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X111"/>
+  <autoFilter ref="A1:Y103"/>
   <hyperlinks>
     <hyperlink ref="G92" r:id="rId1"/>
     <hyperlink ref="G96" r:id="rId2" location="data/PX"/>
+    <hyperlink ref="G91" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>